<commit_message>
Added in starting milestones, timeline, and effort matrix
</commit_message>
<xml_diff>
--- a/Effort_Matrix.xlsx
+++ b/Effort_Matrix.xlsx
@@ -1,25 +1,119 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmful\Downloads\senior_design\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751B85EE-F649-4022-8A61-3250ED114B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+  <si>
+    <t>Task Description</t>
+  </si>
+  <si>
+    <t>Primary Responsibility</t>
+  </si>
+  <si>
+    <t>Specify Game Mechanics</t>
+  </si>
+  <si>
+    <t>Develop Game Prototype</t>
+  </si>
+  <si>
+    <t>Integrate Unity and RL Framework</t>
+  </si>
+  <si>
+    <t>Design RL Agent Architecture</t>
+  </si>
+  <si>
+    <t>Implement RL Agent</t>
+  </si>
+  <si>
+    <t>Create Training Environment</t>
+  </si>
+  <si>
+    <t>Define Training Scenarios</t>
+  </si>
+  <si>
+    <t>Train RL Agent</t>
+  </si>
+  <si>
+    <t>Evaluate RL Agent</t>
+  </si>
+  <si>
+    <t>Refine Game Mechanics</t>
+  </si>
+  <si>
+    <t>Enhance Game Features</t>
+  </si>
+  <si>
+    <t>Update RL Agent</t>
+  </si>
+  <si>
+    <t>Test Gameplay Experience</t>
+  </si>
+  <si>
+    <t>Document Project Progress</t>
+  </si>
+  <si>
+    <t>Project Presentation and Reporting</t>
+  </si>
+  <si>
+    <t>Trevor Darst (Game Developer)</t>
+  </si>
+  <si>
+    <t>Roshan Krishnan (Machine Learning Engineer)</t>
+  </si>
+  <si>
+    <t>Noah Hienen (Game Designer)</t>
+  </si>
+  <si>
+    <t>Noah Hienen (Game Designer/Software Engineer)</t>
+  </si>
+  <si>
+    <t>Noah Heinen (Software Engineer)</t>
+  </si>
+  <si>
+    <t>Grant Fullenkamp (Project Supervisor)</t>
+  </si>
+  <si>
+    <t>Total Effort (%/20 = Hours):</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +425,425 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="28.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.05859375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.52734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.17578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="1">
+        <f>SUM(C2:F2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="1">
+        <f>SUM(C3:F3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G4" s="1">
+        <f>SUM(C4:F4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
+        <f>SUM(C5:F5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G6" s="1">
+        <f>SUM(C6:F6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="1">
+        <f>SUM(C7:F7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G8" s="1">
+        <f>SUM(C8:F8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G9" s="1">
+        <f>SUM(C9:F9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <f>SUM(C10:F10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G11" s="1">
+        <f>SUM(C11:F11)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G12" s="1">
+        <f>SUM(C12:F12)</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G13" s="1">
+        <f>SUM(C13:F13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="1">
+        <f>SUM(C14:F14)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G15" s="1">
+        <f>SUM(C15:F15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G16" s="1">
+        <f>SUM(C16:F16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="C17" s="1">
+        <f>SUM(C2:C16)</f>
+        <v>4.3</v>
+      </c>
+      <c r="D17" s="1">
+        <f>SUM(D2:D16)</f>
+        <v>3.6000000000000005</v>
+      </c>
+      <c r="E17" s="1">
+        <f>SUM(E2:E16)</f>
+        <v>3.6</v>
+      </c>
+      <c r="F17" s="1">
+        <f>SUM(F2:F16)</f>
+        <v>3.6000000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.5">
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <f>C17*20</f>
+        <v>86</v>
+      </c>
+      <c r="D18">
+        <f>D17*20</f>
+        <v>72.000000000000014</v>
+      </c>
+      <c r="E18">
+        <f>E17*20</f>
+        <v>72</v>
+      </c>
+      <c r="F18">
+        <f>F17*20</f>
+        <v>72.000000000000014</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>